<commit_message>
Started enhancing neuromechanical simulator to read neuron and synapse data files.
</commit_message>
<xml_diff>
--- a/Code/Matlab/Quadruped_Simulation/Quadruped_Simulation_Framework/Utilities/Robot_Data/Joint_Data.xlsx
+++ b/Code/Matlab/Quadruped_Simulation/Quadruped_Simulation_Framework/Utilities/Robot_Data/Joint_Data.xlsx
@@ -1,24 +1,33 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24729"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\USER\Documents\GitHub\Quadruped_Robot\Code\Matlab\Solutions\Main\Precomputed_Network_Simulation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Cody Scharzenberger\Documents\GitHub\Quadruped_Robot\Code\Matlab\Quadruped_Simulation\Quadruped_Simulation_Framework\Utilities\Robot_Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90DE5A44-7A6A-4CEA-AEC1-DF79FD18FD51}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA08EFC7-0595-484E-86F5-8EC5BE4C2032}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{D94899F0-6C00-4EFE-A0D1-18351498C7BD}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{D94899F0-6C00-4EFE-A0D1-18351498C7BD}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -426,13 +435,13 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="6">
@@ -756,7 +765,7 @@
   <dimension ref="A1:Z17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="AB3" sqref="AB3"/>
+      <selection activeCell="N25" sqref="N25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -795,10 +804,10 @@
       <c r="D1" s="52" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="53" t="s">
+      <c r="E1" s="51" t="s">
         <v>22</v>
       </c>
-      <c r="F1" s="53" t="s">
+      <c r="F1" s="51" t="s">
         <v>23</v>
       </c>
       <c r="G1" s="52" t="s">
@@ -808,29 +817,29 @@
         <v>34</v>
       </c>
       <c r="I1" s="52"/>
-      <c r="J1" s="51" t="s">
+      <c r="J1" s="53" t="s">
         <v>5</v>
       </c>
-      <c r="K1" s="51"/>
-      <c r="L1" s="51"/>
-      <c r="M1" s="51"/>
-      <c r="N1" s="51"/>
-      <c r="O1" s="51"/>
-      <c r="P1" s="51" t="s">
+      <c r="K1" s="53"/>
+      <c r="L1" s="53"/>
+      <c r="M1" s="53"/>
+      <c r="N1" s="53"/>
+      <c r="O1" s="53"/>
+      <c r="P1" s="53" t="s">
         <v>28</v>
       </c>
-      <c r="Q1" s="51"/>
-      <c r="R1" s="51"/>
-      <c r="S1" s="51" t="s">
+      <c r="Q1" s="53"/>
+      <c r="R1" s="53"/>
+      <c r="S1" s="53" t="s">
         <v>26</v>
       </c>
-      <c r="T1" s="51"/>
-      <c r="U1" s="51"/>
-      <c r="V1" s="51" t="s">
+      <c r="T1" s="53"/>
+      <c r="U1" s="53"/>
+      <c r="V1" s="53" t="s">
         <v>27</v>
       </c>
-      <c r="W1" s="51"/>
-      <c r="X1" s="51"/>
+      <c r="W1" s="53"/>
+      <c r="X1" s="53"/>
       <c r="Y1" s="49" t="s">
         <v>35</v>
       </c>
@@ -843,8 +852,8 @@
       <c r="B2" s="52"/>
       <c r="C2" s="52"/>
       <c r="D2" s="52"/>
-      <c r="E2" s="53"/>
-      <c r="F2" s="53"/>
+      <c r="E2" s="51"/>
+      <c r="F2" s="51"/>
       <c r="G2" s="52"/>
       <c r="H2" s="1" t="s">
         <v>32</v>
@@ -852,18 +861,18 @@
       <c r="I2" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="J2" s="51" t="s">
+      <c r="J2" s="53" t="s">
         <v>2</v>
       </c>
-      <c r="K2" s="51"/>
-      <c r="L2" s="51" t="s">
+      <c r="K2" s="53"/>
+      <c r="L2" s="53" t="s">
         <v>3</v>
       </c>
-      <c r="M2" s="51"/>
-      <c r="N2" s="51" t="s">
+      <c r="M2" s="53"/>
+      <c r="N2" s="53" t="s">
         <v>4</v>
       </c>
-      <c r="O2" s="51"/>
+      <c r="O2" s="53"/>
       <c r="P2" s="2" t="s">
         <v>2</v>
       </c>
@@ -2199,6 +2208,11 @@
     </row>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:C2"/>
+    <mergeCell ref="D1:D2"/>
+    <mergeCell ref="E1:E2"/>
     <mergeCell ref="Z1:Z2"/>
     <mergeCell ref="F1:F2"/>
     <mergeCell ref="G1:G2"/>
@@ -2206,11 +2220,6 @@
     <mergeCell ref="L2:M2"/>
     <mergeCell ref="N2:O2"/>
     <mergeCell ref="H1:I1"/>
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:C2"/>
-    <mergeCell ref="D1:D2"/>
-    <mergeCell ref="E1:E2"/>
     <mergeCell ref="Y1:Y2"/>
     <mergeCell ref="P1:R1"/>
     <mergeCell ref="S1:U1"/>

</xml_diff>